<commit_message>
python is on drugs
</commit_message>
<xml_diff>
--- a/resources/btc-atr.xlsx
+++ b/resources/btc-atr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomsr\Documents\Code\production\pypi\rolling-ta\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C795CC73-1EA9-4B91-85B3-CAEA5AAD6361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B1C264-0E1B-4F7D-8261-EB8FBC478EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-8565" windowWidth="16410" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28590" yWindow="-8955" windowWidth="16410" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -369,8 +369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,8 +392,8 @@
         <v>13319</v>
       </c>
       <c r="E1">
-        <f>ROUND(B1-C1, 6)</f>
-        <v>56.8</v>
+        <f>B1-C1</f>
+        <v>56.799999999999272</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -410,7 +410,7 @@
         <v>13319</v>
       </c>
       <c r="E2">
-        <f>MAX(B2-C2, ABS(B2-D1), D1-C2)</f>
+        <f>MAX(B2 - C2, ABS(B2 - D1), ABS(D1 - C2))</f>
         <v>0</v>
       </c>
     </row>
@@ -428,7 +428,7 @@
         <v>13346.2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E66" si="0">MAX(B3-C3, ABS(B3-D2), D2-C3)</f>
+        <f t="shared" ref="E3:E66" si="0">MAX(B3 - C3, ABS(B3 - D2), ABS(D2 - C3))</f>
         <v>50.299999999999272</v>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="F14">
         <f>AVERAGE(E1:E14)</f>
-        <v>35.821428571428235</v>
+        <v>35.821428571428179</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -653,7 +653,7 @@
       </c>
       <c r="F15">
         <f>((F14 * 13) + E15) /14</f>
-        <v>34.855612244897593</v>
+        <v>34.855612244897543</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -675,7 +675,7 @@
       </c>
       <c r="F16">
         <f t="shared" ref="F16:F79" si="1">((F15 * 13) + E16) /14</f>
-        <v>34.001639941690591</v>
+        <v>34.001639941690549</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -697,7 +697,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>31.572951374426975</v>
+        <v>31.572951374426939</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -719,7 +719,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>31.182026276253644</v>
+        <v>31.182026276253612</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -741,7 +741,7 @@
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>31.683310113664152</v>
+        <v>31.683310113664124</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>29.420216534116715</v>
+        <v>29.420216534116687</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -785,7 +785,7 @@
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>27.318772495965522</v>
+        <v>27.318772495965497</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -807,7 +807,7 @@
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>29.231717317682296</v>
+        <v>29.231717317682271</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -829,7 +829,7 @@
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>35.236594652133512</v>
+        <v>35.236594652133483</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -851,7 +851,7 @@
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>34.919695034124054</v>
+        <v>34.919695034124025</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -873,7 +873,7 @@
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>35.246859674543764</v>
+        <v>35.246859674543735</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -895,7 +895,7 @@
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>34.472083983504895</v>
+        <v>34.472083983504874</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -917,7 +917,7 @@
       </c>
       <c r="F27">
         <f t="shared" si="1"/>
-        <v>34.331220841825974</v>
+        <v>34.331220841825953</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -939,7 +939,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>33.600419353124146</v>
+        <v>33.600419353124124</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
       </c>
       <c r="F29">
         <f t="shared" si="1"/>
-        <v>35.114675113615228</v>
+        <v>35.114675113615206</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -983,7 +983,7 @@
       </c>
       <c r="F30">
         <f t="shared" si="1"/>
-        <v>35.399341176928452</v>
+        <v>35.399341176928431</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="F31">
         <f t="shared" si="1"/>
-        <v>35.749388235719358</v>
+        <v>35.749388235719337</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1027,7 +1027,7 @@
       </c>
       <c r="F32">
         <f t="shared" si="1"/>
-        <v>37.531574790310756</v>
+        <v>37.531574790310735</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="1"/>
-        <v>41.53646230528846</v>
+        <v>41.536462305288431</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1071,7 +1071,7 @@
       </c>
       <c r="F34">
         <f t="shared" si="1"/>
-        <v>39.205286426339391</v>
+        <v>39.205286426339356</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="F35">
         <f t="shared" si="1"/>
-        <v>38.433480253029536</v>
+        <v>38.433480253029508</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="F36">
         <f t="shared" si="1"/>
-        <v>38.009660234956002</v>
+        <v>38.009660234955973</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="F37">
         <f t="shared" si="1"/>
-        <v>37.087541646744889</v>
+        <v>37.087541646744853</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="F38">
         <f t="shared" si="1"/>
-        <v>35.445574386263139</v>
+        <v>35.445574386263104</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="F39">
         <f t="shared" si="1"/>
-        <v>32.9137476443872</v>
+        <v>32.913747644387165</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1203,7 +1203,7 @@
       </c>
       <c r="F40">
         <f t="shared" si="1"/>
-        <v>31.348479955502398</v>
+        <v>31.348479955502366</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="F41">
         <f t="shared" si="1"/>
-        <v>30.980731387252149</v>
+        <v>30.980731387252121</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1247,7 +1247,7 @@
       </c>
       <c r="F42">
         <f t="shared" si="1"/>
-        <v>31.553536288162711</v>
+        <v>31.553536288162686</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1269,7 +1269,7 @@
       </c>
       <c r="F43">
         <f t="shared" si="1"/>
-        <v>32.09256941043683</v>
+        <v>32.092569410436809</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="F44">
         <f t="shared" si="1"/>
-        <v>35.085957309691345</v>
+        <v>35.085957309691324</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="F45">
         <f t="shared" si="1"/>
-        <v>35.508388930427678</v>
+        <v>35.508388930427657</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1335,7 +1335,7 @@
       </c>
       <c r="F46">
         <f t="shared" si="1"/>
-        <v>33.786361149682818</v>
+        <v>33.786361149682797</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="F47">
         <f t="shared" si="1"/>
-        <v>33.42304963899111</v>
+        <v>33.423049638991088</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="F48">
         <f t="shared" si="1"/>
-        <v>34.307117521920397</v>
+        <v>34.307117521920375</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="F49">
         <f t="shared" si="1"/>
-        <v>34.349466270354625</v>
+        <v>34.349466270354604</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="F50">
         <f t="shared" si="1"/>
-        <v>34.245932965329267</v>
+        <v>34.245932965329253</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1445,7 +1445,7 @@
       </c>
       <c r="F51">
         <f t="shared" si="1"/>
-        <v>32.199794896377206</v>
+        <v>32.199794896377192</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1467,7 +1467,7 @@
       </c>
       <c r="F52">
         <f t="shared" si="1"/>
-        <v>34.978380975207429</v>
+        <v>34.978380975207422</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1792,7 +1792,7 @@
         <v>13668.4</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E130" si="2">MAX(B67-C67, ABS(B67-D66), D66-C67)</f>
+        <f t="shared" ref="E67:E130" si="2">MAX(B67 - C67, ABS(B67 - D66), ABS(D66 - C67))</f>
         <v>14.199999999998909</v>
       </c>
       <c r="F67">
@@ -3200,7 +3200,7 @@
         <v>13706.6</v>
       </c>
       <c r="E131">
-        <f t="shared" ref="E131:E194" si="4">MAX(B131-C131, ABS(B131-D130), D130-C131)</f>
+        <f t="shared" ref="E131:E194" si="4">MAX(B131 - C131, ABS(B131 - D130), ABS(D130 - C131))</f>
         <v>0</v>
       </c>
       <c r="F131">
@@ -4608,7 +4608,7 @@
         <v>13731.3</v>
       </c>
       <c r="E195">
-        <f t="shared" ref="E195:E200" si="6">MAX(B195-C195, ABS(B195-D194), D194-C195)</f>
+        <f t="shared" ref="E195:E200" si="6">MAX(B195 - C195, ABS(B195 - D194), ABS(D194 - C195))</f>
         <v>30.199999999998909</v>
       </c>
       <c r="F195">

</xml_diff>

<commit_message>
huge derp on my part
</commit_message>
<xml_diff>
--- a/resources/btc-atr.xlsx
+++ b/resources/btc-atr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomsr\Documents\Code\production\pypi\rolling-ta\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B1C264-0E1B-4F7D-8261-EB8FBC478EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1EFC00-A4C2-476F-BED7-A39BF825986D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28590" yWindow="-8955" windowWidth="16410" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -367,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F200"/>
+  <dimension ref="A1:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,7 +1030,7 @@
         <v>37.531574790310735</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1515671040</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>41.536462305288431</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1515671100</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>39.205286426339356</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1515671160</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>38.433480253029508</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1515671220</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>38.009660234955973</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1515671280</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>37.087541646744853</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1515671340</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>35.445574386263104</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1515671400</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>32.913747644387165</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1515671460</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>31.348479955502366</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1515671520</v>
       </c>
@@ -1227,8 +1227,12 @@
         <f t="shared" si="1"/>
         <v>30.980731387252121</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <f>MAX(B41-C41,ABS(B41-D40),D40-C41)</f>
+        <v>26.199999999998909</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1515671580</v>
       </c>
@@ -1250,7 +1254,7 @@
         <v>31.553536288162686</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1515671640</v>
       </c>
@@ -1272,7 +1276,7 @@
         <v>32.092569410436809</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1515671700</v>
       </c>
@@ -1294,7 +1298,7 @@
         <v>35.085957309691324</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1515671760</v>
       </c>
@@ -1316,7 +1320,7 @@
         <v>35.508388930427657</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1515671820</v>
       </c>
@@ -1338,7 +1342,7 @@
         <v>33.786361149682797</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1515671880</v>
       </c>
@@ -1360,7 +1364,7 @@
         <v>33.423049638991088</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1515671940</v>
       </c>

</xml_diff>

<commit_message>
added names to evaluate test func to help debug
</commit_message>
<xml_diff>
--- a/resources/btc-atr.xlsx
+++ b/resources/btc-atr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomsr\Documents\Code\production\pypi\rolling-ta\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1EFC00-A4C2-476F-BED7-A39BF825986D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262CFD11-63FE-49B8-87F2-FF9F2FB3665D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28590" yWindow="-8955" windowWidth="16410" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -367,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G200"/>
+  <dimension ref="A1:F200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,6 +395,9 @@
         <f>B1-C1</f>
         <v>56.799999999999272</v>
       </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -413,6 +416,9 @@
         <f>MAX(B2 - C2, ABS(B2 - D1), ABS(D1 - C2))</f>
         <v>0</v>
       </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -431,6 +437,9 @@
         <f t="shared" ref="E3:E66" si="0">MAX(B3 - C3, ABS(B3 - D2), ABS(D2 - C3))</f>
         <v>50.299999999999272</v>
       </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -449,6 +458,9 @@
         <f t="shared" si="0"/>
         <v>9.9999999998544808E-2</v>
       </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -467,6 +479,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -485,6 +500,9 @@
         <f t="shared" si="0"/>
         <v>73.299999999999272</v>
       </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -503,6 +521,9 @@
         <f t="shared" si="0"/>
         <v>22.099999999998545</v>
       </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -521,6 +542,9 @@
         <f t="shared" si="0"/>
         <v>44.799999999999272</v>
       </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -539,6 +563,9 @@
         <f t="shared" si="0"/>
         <v>81.899999999999636</v>
       </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -557,6 +584,9 @@
         <f t="shared" si="0"/>
         <v>37.5</v>
       </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -575,6 +605,9 @@
         <f t="shared" si="0"/>
         <v>33.799999999999272</v>
       </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -593,6 +626,9 @@
         <f t="shared" si="0"/>
         <v>53.800000000001091</v>
       </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -611,6 +647,9 @@
         <f t="shared" si="0"/>
         <v>17.899999999999636</v>
       </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1030,7 +1069,7 @@
         <v>37.531574790310735</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1515671040</v>
       </c>
@@ -1052,7 +1091,7 @@
         <v>41.536462305288431</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1515671100</v>
       </c>
@@ -1074,7 +1113,7 @@
         <v>39.205286426339356</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1515671160</v>
       </c>
@@ -1096,7 +1135,7 @@
         <v>38.433480253029508</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1515671220</v>
       </c>
@@ -1118,7 +1157,7 @@
         <v>38.009660234955973</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1515671280</v>
       </c>
@@ -1140,7 +1179,7 @@
         <v>37.087541646744853</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1515671340</v>
       </c>
@@ -1162,7 +1201,7 @@
         <v>35.445574386263104</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1515671400</v>
       </c>
@@ -1184,7 +1223,7 @@
         <v>32.913747644387165</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1515671460</v>
       </c>
@@ -1206,7 +1245,7 @@
         <v>31.348479955502366</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1515671520</v>
       </c>
@@ -1227,12 +1266,8 @@
         <f t="shared" si="1"/>
         <v>30.980731387252121</v>
       </c>
-      <c r="G41">
-        <f>MAX(B41-C41,ABS(B41-D40),D40-C41)</f>
-        <v>26.199999999998909</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1515671580</v>
       </c>
@@ -1254,7 +1289,7 @@
         <v>31.553536288162686</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1515671640</v>
       </c>
@@ -1276,7 +1311,7 @@
         <v>32.092569410436809</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1515671700</v>
       </c>
@@ -1298,7 +1333,7 @@
         <v>35.085957309691324</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1515671760</v>
       </c>
@@ -1320,7 +1355,7 @@
         <v>35.508388930427657</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1515671820</v>
       </c>
@@ -1342,7 +1377,7 @@
         <v>33.786361149682797</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1515671880</v>
       </c>
@@ -1364,7 +1399,7 @@
         <v>33.423049638991088</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1515671940</v>
       </c>

</xml_diff>